<commit_message>
Testing values, Min Value: 21276.0
</commit_message>
<xml_diff>
--- a/distance_matrix.xlsx
+++ b/distance_matrix.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\Air_semestr_5\BO2\projekt\BO2_Evolutionary_Algorithm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szyme\Documents\Studia\V semestr\BO_2\projekt\BO2_Evolutionary_Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133433FE-7D0B-4290-AD7D-665B090BD74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="1">
   <si>
     <t>inf</t>
   </si>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,16 +343,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -372,124 +371,218 @@
       <c r="F1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>25</v>
       </c>
       <c r="E2">
-        <v>1000</v>
+        <v>40</v>
       </c>
       <c r="F2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>65</v>
+      </c>
+      <c r="H2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>1000</v>
+        <v>34</v>
       </c>
       <c r="F3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="G3">
+        <v>58</v>
+      </c>
+      <c r="H3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1000</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>1000</v>
+        <v>25</v>
       </c>
       <c r="F4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1000</v>
+        <v>25</v>
       </c>
       <c r="B5">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1000</v>
+        <v>40</v>
       </c>
       <c r="B6">
-        <v>1000</v>
+        <v>34</v>
       </c>
       <c r="C6">
-        <v>1000</v>
+        <v>25</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>26</v>
+      </c>
+      <c r="H6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="B7">
-        <v>1000</v>
+        <v>45</v>
       </c>
       <c r="C7">
-        <v>1000</v>
+        <v>37</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>26</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>65</v>
+      </c>
+      <c r="B8">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>38</v>
+      </c>
+      <c r="E8">
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>75</v>
+      </c>
+      <c r="B9">
+        <v>72</v>
+      </c>
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="D9">
+        <v>54</v>
+      </c>
+      <c r="E9">
+        <v>42</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>